<commit_message>
new  test scenarios added
</commit_message>
<xml_diff>
--- a/Test Data/Sav-Scenarios.xlsx
+++ b/Test Data/Sav-Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnithaB\git\Saviynt\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB84C13B-105F-4FEC-940C-8490E26BB2DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68748126-36AA-4AF6-951F-3585EDFE335E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{5DD385BD-E735-4168-8DF3-DF7C7B7F794E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>ROLES</t>
   </si>
@@ -86,17 +86,68 @@
     <t>thmefx</t>
   </si>
   <si>
-    <t>New approver</t>
-  </si>
-  <si>
     <t>sisor7</t>
+  </si>
+  <si>
+    <t>shintj</t>
+  </si>
+  <si>
+    <t>DZMP8A</t>
+  </si>
+  <si>
+    <t>Requestor</t>
+  </si>
+  <si>
+    <t>End User</t>
+  </si>
+  <si>
+    <t>User Names For Applicaton Specific Roles</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>GD:PL_PO_INVOICE_RELEASE</t>
+  </si>
+  <si>
+    <t>GD:PL_AP_ONLY_PAYMENT_RESTRICT</t>
+  </si>
+  <si>
+    <t>LVC:C:PLFI:BAL_SHT_COST_CONTRO</t>
+  </si>
+  <si>
+    <t>GD:PL_CO_PROFIT_COST_CENTER_M</t>
+  </si>
+  <si>
+    <t>R10,R11,R12,R13</t>
+  </si>
+  <si>
+    <t>New approver(ER)</t>
+  </si>
+  <si>
+    <t>New approver(ASP)</t>
+  </si>
+  <si>
+    <t>basqdp</t>
+  </si>
+  <si>
+    <t>dah1nu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +175,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +201,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -157,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -168,6 +231,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,15 +550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E49D47-FC05-4B6E-B2A1-08E93041445E}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -530,39 +598,44 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="3"/>
+    </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="5"/>
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="5"/>
     </row>
@@ -571,23 +644,101 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new test cases for L2 manager added.
</commit_message>
<xml_diff>
--- a/Test Data/Sav-Scenarios.xlsx
+++ b/Test Data/Sav-Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnithaB\git\Saviynt\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E046B6-D2E4-4AB0-94F1-D15285AF536F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614E8543-E4A2-47EB-9AA1-D77EF5C53900}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5DD385BD-E735-4168-8DF3-DF7C7B7F794E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>ROLES</t>
   </si>
@@ -154,13 +154,25 @@
   </si>
   <si>
     <t>L2TEST13</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>TrainingWorkOrderApprover</t>
+  </si>
+  <si>
+    <t>RGTST01</t>
+  </si>
+  <si>
+    <t>Upstream|AFT|Alaska|Reporting - Standard User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +205,12 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -233,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -247,6 +265,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -565,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E49D47-FC05-4B6E-B2A1-08E93041445E}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -762,15 +783,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0541D8-32FD-43B3-B9C7-705CA7A986D3}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -793,6 +814,26 @@
         <v>40</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>